<commit_message>
feat: VERSION 1.2 CON LOS CAMBIOS AL FORMATO DE CONTROL DE PRODUCTO EN BULTO Y CAMBIOS EN EL GIT PARA IGNORAR GENERADOS
</commit_message>
<xml_diff>
--- a/archivos/formularios/formulario7.xlsx
+++ b/archivos/formularios/formulario7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fmt\archivos\formularios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.mora\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3451090E-0061-4C36-9D55-E10BE22AEED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66CB5D3-E07B-4384-A853-7FEDF49A094C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="-11640" windowWidth="20730" windowHeight="11040" xr2:uid="{32DE228C-E90D-4752-987D-C3058691DA33}"/>
+    <workbookView xWindow="12852" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{32DE228C-E90D-4752-987D-C3058691DA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -604,9 +604,6 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,6 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,28 +1012,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B227E9F2-CFE9-4186-861C-B5A120C9CF8A}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.08984375" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" customWidth="1"/>
-    <col min="12" max="12" width="9.90625" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1062,7 +1060,7 @@
       </c>
       <c r="Q1" s="41"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="27"/>
       <c r="C2" s="35"/>
@@ -1085,7 +1083,7 @@
       </c>
       <c r="Q2" s="41"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="27"/>
       <c r="C3" s="35"/>
@@ -1108,7 +1106,7 @@
       </c>
       <c r="Q3" s="41"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
       <c r="B4" s="27"/>
       <c r="C4" s="35"/>
@@ -1131,7 +1129,7 @@
       </c>
       <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -1143,10 +1141,10 @@
       <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="10" t="s">
         <v>17</v>
       </c>
@@ -1154,15 +1152,20 @@
       <c r="L5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="18">
+        <v>0.15</v>
+      </c>
       <c r="N5" s="19"/>
       <c r="O5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-    </row>
-    <row r="6" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P5" s="46">
+        <f>K5+M5</f>
+        <v>0.15</v>
+      </c>
+      <c r="Q5" s="46"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
@@ -1238,7 +1241,7 @@
       </c>
       <c r="Q7" s="39"/>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -1260,7 +1263,7 @@
       <c r="P8" s="22"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1276,13 +1279,13 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="22" t="e">
-        <f t="shared" ref="O9:O28" si="0">AVERAGE(D9:M9)</f>
+        <f t="shared" ref="O9:O72" si="0">AVERAGE(D9:M9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1304,7 +1307,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1326,7 +1329,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1348,7 +1351,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1370,7 +1373,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1392,7 +1395,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1414,7 +1417,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1436,7 +1439,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1458,7 +1461,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1480,7 +1483,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1502,7 +1505,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1524,7 +1527,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1546,7 +1549,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1568,7 +1571,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1590,7 +1593,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1612,7 +1615,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1634,7 +1637,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1656,7 +1659,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1678,7 +1681,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -1700,8 +1703,3140 @@
       <c r="P28" s="23"/>
       <c r="Q28" s="7"/>
     </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O29" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O30" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O31" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O33" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O34" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O35" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O36" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O37" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O38" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O39" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O40" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O41" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O42" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O43" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O44" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O45" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O46" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O47" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O48" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O49" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O50" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O51" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O52" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O53" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O54" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O55" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O56" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O57" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O58" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O59" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O60" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O61" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O62" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O63" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O64" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O65" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O66" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O67" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O68" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O69" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O70" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O71" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O72" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O73" s="22" t="e">
+        <f t="shared" ref="O73:O136" si="1">AVERAGE(D73:M73)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O74" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O75" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O76" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O77" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O78" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O79" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O80" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O81" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O82" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O83" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O84" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O85" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O86" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O87" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O88" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O89" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O90" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O91" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O92" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O93" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O94" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O95" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O96" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O97" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O98" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O99" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O100" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O101" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O102" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O103" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O104" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O105" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O106" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O107" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O108" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O109" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O110" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O111" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O112" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O113" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O114" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O115" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O116" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O117" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O118" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O119" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O120" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O121" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O122" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O123" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O124" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O125" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O126" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O127" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O128" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O129" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O130" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O131" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O132" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O133" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O134" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O135" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O136" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O137" s="22" t="e">
+        <f t="shared" ref="O137:O200" si="2">AVERAGE(D137:M137)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="138" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O138" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="139" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O139" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="140" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O140" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="141" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O141" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="142" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O142" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="143" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O143" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="144" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O144" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="145" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O145" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="146" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O146" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="147" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O147" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="148" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O148" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="149" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O149" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="150" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O150" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="151" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O151" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="152" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O152" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="153" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O153" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="154" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O154" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="155" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O155" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="156" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O156" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="157" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O157" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="158" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O158" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="159" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O159" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="160" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O160" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="161" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O161" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="162" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O162" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="163" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O163" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="164" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O164" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="165" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O165" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="166" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O166" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="167" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O167" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="168" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O168" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="169" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O169" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="170" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O170" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="171" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O171" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="172" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O172" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="173" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O173" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="174" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O174" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="175" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O175" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="176" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O176" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="177" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O177" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="178" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O178" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="179" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O179" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="180" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O180" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="181" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O181" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="182" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O182" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="183" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O183" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="184" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O184" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="185" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O185" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="186" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O186" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="187" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O187" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="188" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O188" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="189" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O189" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="190" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O190" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="191" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O191" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="192" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O192" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="193" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O193" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="194" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O194" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="195" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O195" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="196" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O196" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="197" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O197" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="198" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O198" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="199" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O199" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="200" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O200" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="201" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O201" s="22" t="e">
+        <f t="shared" ref="O201:O264" si="3">AVERAGE(D201:M201)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="202" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O202" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="203" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O203" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="204" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O204" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="205" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O205" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="206" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O206" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="207" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O207" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="208" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O208" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="209" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O209" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="210" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O210" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="211" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O211" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="212" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O212" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="213" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O213" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="214" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O214" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="215" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O215" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="216" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O216" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="217" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O217" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="218" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O218" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="219" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O219" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="220" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O220" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="221" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O221" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="222" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O222" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="223" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O223" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="224" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O224" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="225" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O225" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="226" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O226" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="227" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O227" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="228" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O228" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="229" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O229" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="230" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O230" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="231" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O231" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="232" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O232" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="233" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O233" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="234" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O234" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="235" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O235" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="236" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O236" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="237" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O237" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="238" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O238" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="239" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O239" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="240" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O240" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="241" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O241" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="242" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O242" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="243" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O243" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="244" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O244" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="245" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O245" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="246" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O246" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="247" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O247" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="248" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O248" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="249" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O249" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="250" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O250" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="251" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O251" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="252" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O252" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="253" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O253" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="254" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O254" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="255" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O255" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="256" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O256" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="257" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O257" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="258" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O258" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="259" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O259" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="260" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O260" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="261" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O261" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="262" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O262" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="263" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O263" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="264" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O264" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="265" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O265" s="22" t="e">
+        <f t="shared" ref="O265:O328" si="4">AVERAGE(D265:M265)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="266" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O266" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="267" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O267" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="268" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O268" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="269" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O269" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="270" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O270" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="271" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O271" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="272" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O272" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="273" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O273" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="274" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O274" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="275" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O275" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="276" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O276" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="277" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O277" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="278" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O278" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="279" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O279" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="280" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O280" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="281" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O281" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="282" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O282" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="283" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O283" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="284" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O284" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="285" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O285" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="286" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O286" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="287" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O287" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="288" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O288" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="289" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O289" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="290" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O290" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="291" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O291" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="292" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O292" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="293" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O293" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="294" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O294" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="295" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O295" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="296" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O296" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="297" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O297" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="298" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O298" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="299" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O299" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="300" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O300" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="301" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O301" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="302" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O302" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="303" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O303" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="304" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O304" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="305" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O305" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="306" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O306" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="307" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O307" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="308" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O308" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="309" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O309" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="310" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O310" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="311" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O311" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="312" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O312" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="313" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O313" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="314" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O314" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="315" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O315" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="316" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O316" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="317" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O317" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="318" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O318" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="319" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O319" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="320" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O320" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="321" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O321" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="322" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O322" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="323" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O323" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="324" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O324" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="325" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O325" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="326" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O326" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="327" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O327" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="328" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O328" s="22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="329" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O329" s="22" t="e">
+        <f t="shared" ref="O329:O392" si="5">AVERAGE(D329:M329)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="330" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O330" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="331" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O331" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="332" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O332" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="333" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O333" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="334" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O334" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="335" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O335" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="336" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O336" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="337" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O337" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="338" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O338" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="339" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O339" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="340" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O340" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="341" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O341" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="342" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O342" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="343" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O343" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="344" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O344" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="345" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O345" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="346" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O346" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="347" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O347" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="348" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O348" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="349" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O349" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="350" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O350" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="351" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O351" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="352" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O352" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="353" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O353" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="354" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O354" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="355" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O355" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="356" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O356" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="357" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O357" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="358" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O358" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="359" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O359" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="360" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O360" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="361" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O361" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="362" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O362" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="363" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O363" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="364" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O364" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="365" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O365" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="366" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O366" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="367" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O367" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="368" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O368" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="369" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O369" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="370" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O370" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="371" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O371" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="372" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O372" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="373" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O373" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="374" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O374" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="375" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O375" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="376" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O376" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="377" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O377" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="378" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O378" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="379" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O379" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="380" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O380" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="381" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O381" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="382" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O382" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="383" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O383" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="384" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O384" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="385" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O385" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="386" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O386" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="387" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O387" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="388" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O388" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="389" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O389" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="390" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O390" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="391" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O391" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="392" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O392" s="22" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="393" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O393" s="22" t="e">
+        <f t="shared" ref="O393:O456" si="6">AVERAGE(D393:M393)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="394" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O394" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="395" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O395" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="396" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O396" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="397" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O397" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="398" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O398" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="399" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O399" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="400" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O400" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="401" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O401" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="402" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O402" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="403" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O403" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="404" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O404" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="405" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O405" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="406" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O406" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="407" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O407" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="408" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O408" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="409" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O409" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="410" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O410" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="411" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O411" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="412" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O412" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="413" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O413" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="414" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O414" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="415" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O415" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="416" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O416" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="417" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O417" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="418" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O418" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="419" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O419" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="420" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O420" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="421" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O421" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="422" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O422" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="423" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O423" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="424" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O424" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="425" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O425" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="426" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O426" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="427" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O427" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="428" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O428" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="429" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O429" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="430" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O430" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="431" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O431" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="432" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O432" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="433" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O433" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="434" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O434" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="435" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O435" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="436" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O436" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="437" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O437" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="438" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O438" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="439" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O439" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="440" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O440" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="441" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O441" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="442" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O442" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="443" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O443" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="444" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O444" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="445" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O445" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="446" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O446" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="447" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O447" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="448" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O448" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="449" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O449" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="450" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O450" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="451" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O451" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="452" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O452" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="453" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O453" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="454" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O454" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="455" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O455" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="456" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O456" s="22" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="457" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O457" s="22" t="e">
+        <f t="shared" ref="O457:O520" si="7">AVERAGE(D457:M457)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="458" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O458" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="459" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O459" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="460" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O460" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="461" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O461" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="462" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O462" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="463" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O463" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="464" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O464" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="465" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O465" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="466" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O466" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="467" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O467" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="468" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O468" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="469" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O469" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="470" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O470" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="471" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O471" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="472" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O472" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="473" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O473" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="474" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O474" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="475" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O475" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="476" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O476" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="477" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O477" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="478" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O478" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="479" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O479" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="480" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O480" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="481" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O481" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="482" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O482" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="483" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O483" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="484" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O484" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="485" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O485" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="486" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O486" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="487" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O487" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="488" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O488" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="489" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O489" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="490" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O490" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="491" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O491" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="492" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O492" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="493" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O493" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="494" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O494" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="495" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O495" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="496" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O496" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="497" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O497" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="498" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O498" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="499" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O499" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="500" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O500" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="501" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O501" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="502" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O502" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="503" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O503" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="504" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O504" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="505" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O505" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="506" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O506" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="507" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O507" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="508" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O508" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="509" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O509" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="510" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O510" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="511" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O511" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="512" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O512" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="513" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O513" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="514" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O514" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="515" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O515" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="516" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O516" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="517" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O517" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="518" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O518" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="519" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O519" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="520" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O520" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="521" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O521" s="22" t="e">
+        <f t="shared" ref="O521:O550" si="8">AVERAGE(D521:M521)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="522" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O522" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="523" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O523" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="524" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O524" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="525" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O525" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="526" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O526" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="527" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O527" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="528" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O528" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="529" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O529" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="530" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O530" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="531" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O531" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="532" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O532" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="533" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O533" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="534" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O534" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="535" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O535" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="536" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O536" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="537" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O537" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="538" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O538" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="539" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O539" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="540" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O540" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="541" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O541" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="542" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O542" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="543" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O543" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="544" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O544" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="545" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O545" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="546" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O546" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="547" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O547" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="548" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O548" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="549" spans="15:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O549" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="550" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O550" s="22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="D6:N6"/>
@@ -1709,7 +4844,6 @@
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C6:C7"/>

</xml_diff>